<commit_message>
Deploying to gh-pages from @ IDGRLP/Tumorkonferenzen-IG@94fa9ab9aa815cefc95b378045ad6f1ec55afe45 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-AnmeldeBundleMinimalFreitextLunge.xlsx
+++ b/StructureDefinition-AnmeldeBundleMinimalFreitextLunge.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-18T11:11:15+00:00</t>
+    <t>2024-10-31T11:09:37+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -613,7 +613,7 @@
 * Results from operations might involve resources that are not identified.</t>
   </si>
   <si>
-    <t>fullUrl might not be [unique in the context of a resource](bundle.html#bundle-unique). Note that since [FHIR resources do not need to be served through the FHIR API](http://hl7.org/fhir/R4/references.html), the fullURL might be a URN or an absolute URL that does not end with the logical id of the resource (Resource.id). However, but if the fullUrl does look like a RESTful server URL (e.g. meets the [regex](http://hl7.org/fhir/R4/references.html#regex), then the 'id' portion of the fullUrl SHALL end with the Resource.id.
+    <t>fullUrl might not be [unique in the context of a resource](http://hl7.org/fhir/R4/bundle.html#bundle-unique). Note that since [FHIR resources do not need to be served through the FHIR API](http://hl7.org/fhir/R4/references.html), the fullURL might be a URN or an absolute URL that does not end with the logical id of the resource (Resource.id). However, but if the fullUrl does look like a RESTful server URL (e.g. meets the [regex](http://hl7.org/fhir/R4/references.html#regex), then the 'id' portion of the fullUrl SHALL end with the Resource.id.
 Note that the fullUrl is not the same as the canonical URL - it's an absolute url for an endpoint serving the resource (these will happen to have the same value on the canonical server for the resource with the canonical URL).</t>
   </si>
   <si>

</xml_diff>